<commit_message>
Export p75s and calc time incap/offense differently
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -357,7 +357,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ61"/>
+  <dimension ref="A1:AT61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,6 +581,21 @@
           <t>percentOfMatchesNoShow</t>
         </is>
       </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>p75CellsScored</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>p75CellsScoredHigh</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>p75CellsScoredLow</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -706,6 +721,15 @@
       <c r="AQ2" t="n">
         <v>0</v>
       </c>
+      <c r="AR2" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -837,6 +861,15 @@
       <c r="AQ3" t="n">
         <v>0</v>
       </c>
+      <c r="AR3" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -968,6 +1001,15 @@
       <c r="AQ4" t="n">
         <v>0</v>
       </c>
+      <c r="AR4" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1099,6 +1141,15 @@
       <c r="AQ5" t="n">
         <v>0</v>
       </c>
+      <c r="AR5" t="n">
+        <v>9</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>9</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1224,6 +1275,15 @@
       <c r="AQ6" t="n">
         <v>0</v>
       </c>
+      <c r="AR6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>2.7</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1355,6 +1415,15 @@
       <c r="AQ7" t="n">
         <v>0</v>
       </c>
+      <c r="AR7" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1486,6 +1555,15 @@
       <c r="AQ8" t="n">
         <v>0</v>
       </c>
+      <c r="AR8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1617,6 +1695,15 @@
       <c r="AQ9" t="n">
         <v>0</v>
       </c>
+      <c r="AR9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1742,6 +1829,15 @@
       <c r="AQ10" t="n">
         <v>0</v>
       </c>
+      <c r="AR10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1870,6 +1966,15 @@
       <c r="AQ11" t="n">
         <v>0</v>
       </c>
+      <c r="AR11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1995,6 +2100,15 @@
       <c r="AQ12" t="n">
         <v>0</v>
       </c>
+      <c r="AR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -2120,6 +2234,15 @@
       <c r="AQ13" t="n">
         <v>0</v>
       </c>
+      <c r="AR13" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>9.300000000000001</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -2248,6 +2371,15 @@
       <c r="AQ14" t="n">
         <v>0</v>
       </c>
+      <c r="AR14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2379,6 +2511,15 @@
       <c r="AQ15" t="n">
         <v>0</v>
       </c>
+      <c r="AR15" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2510,6 +2651,15 @@
       <c r="AQ16" t="n">
         <v>14</v>
       </c>
+      <c r="AR16" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2641,6 +2791,15 @@
       <c r="AQ17" t="n">
         <v>0</v>
       </c>
+      <c r="AR17" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2772,6 +2931,15 @@
       <c r="AQ18" t="n">
         <v>0</v>
       </c>
+      <c r="AR18" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -2903,6 +3071,15 @@
       <c r="AQ19" t="n">
         <v>0</v>
       </c>
+      <c r="AR19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -3028,6 +3205,15 @@
       <c r="AQ20" t="n">
         <v>0</v>
       </c>
+      <c r="AR20" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -3153,6 +3339,15 @@
       <c r="AQ21" t="n">
         <v>0</v>
       </c>
+      <c r="AR21" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -3284,6 +3479,15 @@
       <c r="AQ22" t="n">
         <v>0</v>
       </c>
+      <c r="AR22" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AS22" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AT22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -3406,6 +3610,15 @@
       <c r="AQ23" t="n">
         <v>0</v>
       </c>
+      <c r="AR23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -3537,6 +3750,15 @@
       <c r="AQ24" t="n">
         <v>0</v>
       </c>
+      <c r="AR24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AS24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -3668,6 +3890,15 @@
       <c r="AQ25" t="n">
         <v>0</v>
       </c>
+      <c r="AR25" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3799,6 +4030,15 @@
       <c r="AQ26" t="n">
         <v>0</v>
       </c>
+      <c r="AR26" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3930,6 +4170,15 @@
       <c r="AQ27" t="n">
         <v>0</v>
       </c>
+      <c r="AR27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -4061,6 +4310,15 @@
       <c r="AQ28" t="n">
         <v>0</v>
       </c>
+      <c r="AR28" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -4189,6 +4447,15 @@
       <c r="AQ29" t="n">
         <v>17</v>
       </c>
+      <c r="AR29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -4320,6 +4587,15 @@
       <c r="AQ30" t="n">
         <v>0</v>
       </c>
+      <c r="AR30" t="n">
+        <v>8</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>8</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -4445,6 +4721,15 @@
       <c r="AQ31" t="n">
         <v>0</v>
       </c>
+      <c r="AR31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -4570,6 +4855,15 @@
       <c r="AQ32" t="n">
         <v>0</v>
       </c>
+      <c r="AR32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -4701,6 +4995,15 @@
       <c r="AQ33" t="n">
         <v>0</v>
       </c>
+      <c r="AR33" t="n">
+        <v>17</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>17</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4832,6 +5135,15 @@
       <c r="AQ34" t="n">
         <v>0</v>
       </c>
+      <c r="AR34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -4963,6 +5275,15 @@
       <c r="AQ35" t="n">
         <v>0</v>
       </c>
+      <c r="AR35" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>3.7</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -5094,6 +5415,15 @@
       <c r="AQ36" t="n">
         <v>0</v>
       </c>
+      <c r="AR36" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AS36" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="AT36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -5225,6 +5555,15 @@
       <c r="AQ37" t="n">
         <v>0</v>
       </c>
+      <c r="AR37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT37" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -5350,6 +5689,15 @@
       <c r="AQ38" t="n">
         <v>0</v>
       </c>
+      <c r="AR38" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS38" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -5481,6 +5829,15 @@
       <c r="AQ39" t="n">
         <v>0</v>
       </c>
+      <c r="AR39" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AS39" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AT39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -5606,6 +5963,15 @@
       <c r="AQ40" t="n">
         <v>0</v>
       </c>
+      <c r="AR40" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AS40" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -5731,6 +6097,15 @@
       <c r="AQ41" t="n">
         <v>0</v>
       </c>
+      <c r="AR41" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AS41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT41" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -5862,6 +6237,15 @@
       <c r="AQ42" t="n">
         <v>0</v>
       </c>
+      <c r="AR42" t="n">
+        <v>6</v>
+      </c>
+      <c r="AS42" t="n">
+        <v>6</v>
+      </c>
+      <c r="AT42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -5993,6 +6377,15 @@
       <c r="AQ43" t="n">
         <v>0</v>
       </c>
+      <c r="AR43" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AS43" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT43" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -6118,6 +6511,15 @@
       <c r="AQ44" t="n">
         <v>0</v>
       </c>
+      <c r="AR44" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AS44" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AT44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -6243,6 +6645,15 @@
       <c r="AQ45" t="n">
         <v>0</v>
       </c>
+      <c r="AR45" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AS45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT45" t="n">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -6374,6 +6785,15 @@
       <c r="AQ46" t="n">
         <v>0</v>
       </c>
+      <c r="AR46" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="AS46" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="AT46" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -6499,6 +6919,15 @@
       <c r="AQ47" t="n">
         <v>0</v>
       </c>
+      <c r="AR47" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AS47" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AT47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -6624,6 +7053,15 @@
       <c r="AQ48" t="n">
         <v>0</v>
       </c>
+      <c r="AR48" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS48" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -6755,6 +7193,15 @@
       <c r="AQ49" t="n">
         <v>0</v>
       </c>
+      <c r="AR49" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="AS49" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="AT49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -6886,6 +7333,15 @@
       <c r="AQ50" t="n">
         <v>0</v>
       </c>
+      <c r="AR50" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="AS50" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AT50" t="n">
+        <v>6.7</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -7017,6 +7473,15 @@
       <c r="AQ51" t="n">
         <v>0</v>
       </c>
+      <c r="AR51" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AS51" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="AT51" t="n">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -7148,6 +7613,15 @@
       <c r="AQ52" t="n">
         <v>0</v>
       </c>
+      <c r="AR52" t="n">
+        <v>10</v>
+      </c>
+      <c r="AS52" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -7279,6 +7753,15 @@
       <c r="AQ53" t="n">
         <v>0</v>
       </c>
+      <c r="AR53" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AS53" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AT53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -7404,6 +7887,15 @@
       <c r="AQ54" t="n">
         <v>0</v>
       </c>
+      <c r="AR54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -7532,6 +8024,15 @@
       <c r="AQ55" t="n">
         <v>0</v>
       </c>
+      <c r="AR55" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="AS55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT55" t="n">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -7663,6 +8164,15 @@
       <c r="AQ56" t="n">
         <v>0</v>
       </c>
+      <c r="AR56" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AS56" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AT56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -7794,6 +8304,15 @@
       <c r="AQ57" t="n">
         <v>0</v>
       </c>
+      <c r="AR57" t="n">
+        <v>8</v>
+      </c>
+      <c r="AS57" t="n">
+        <v>8</v>
+      </c>
+      <c r="AT57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -7925,6 +8444,15 @@
       <c r="AQ58" t="n">
         <v>14</v>
       </c>
+      <c r="AR58" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="AS58" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="AT58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -8047,6 +8575,15 @@
       <c r="AQ59" t="n">
         <v>100</v>
       </c>
+      <c r="AR59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -8172,6 +8709,15 @@
       <c r="AQ60" t="n">
         <v>0</v>
       </c>
+      <c r="AR60" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AS60" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AT60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -8302,6 +8848,15 @@
       </c>
       <c r="AQ61" t="n">
         <v>0</v>
+      </c>
+      <c r="AR61" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="AS61" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="AT61" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>